<commit_message>
added checks to distinguish admin and private user login
</commit_message>
<xml_diff>
--- a/worknest-ui/Manual_Tests.xlsx
+++ b/worknest-ui/Manual_Tests.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riccardo/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC1E0C4-A6F3-2249-AE8D-FA9A23D38385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Manual_Tests.csv" sheetId="1" r:id="rId4"/>
+    <sheet name="Manual_Tests.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="151">
   <si>
     <t>Test case ID</t>
   </si>
@@ -494,35 +503,89 @@
   <si>
     <t>An email reporting the date of the canceld booking, the relative workstation and a confirmation of the successful deleting arrived to the user</t>
   </si>
+  <si>
+    <t>WorkNest Administrator Login #58</t>
+  </si>
+  <si>
+    <t>The user wants to log in with his credentials as an admin</t>
+  </si>
+  <si>
+    <t>Buttons for managing users, companies and bookings are shown</t>
+  </si>
+  <si>
+    <t>The user wants to log in with his credentials as a user</t>
+  </si>
+  <si>
+    <t>&lt;email&gt; and &lt;password&gt; are valid and user type is equal to private user</t>
+  </si>
+  <si>
+    <t>The user login in as an administrator</t>
+  </si>
+  <si>
+    <t>The user login in as a user</t>
+  </si>
+  <si>
+    <t>The administrator user is already registered</t>
+  </si>
+  <si>
+    <t>&lt;email&gt; and &lt;password&gt; are valid and user type is equal to administrator</t>
+  </si>
+  <si>
+    <t>Buttons for managing users, companies and bookings (of all users) are not shown</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF2EB452"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -530,7 +593,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -576,154 +639,152 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="25">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B95F9"/>
           <bgColor rgb="FF5B95F9"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE8F0FE"/>
-          <bgColor rgb="FFE8F0FE"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Manual_Tests.csv-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Manual_Tests.csv-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I30" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:I31">
   <tableColumns count="9">
-    <tableColumn name="Test case ID" id="1"/>
-    <tableColumn name="User Story" id="2"/>
-    <tableColumn name="Test Case Scenario" id="3"/>
-    <tableColumn name="Test Case" id="4"/>
-    <tableColumn name="Pre-conditions" id="5"/>
-    <tableColumn name="Test Steps" id="6"/>
-    <tableColumn name="Test Data" id="7"/>
-    <tableColumn name="Expected Result" id="8"/>
-    <tableColumn name="Match result" id="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test case ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="User Story"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test Case Scenario"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Test Case"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Pre-conditions"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Test Steps"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Test Data"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Expected Result"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Match result"/>
   </tableColumns>
-  <tableStyleInfo name="Manual_Tests.csv-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Manual_Tests.csv-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -913,29 +974,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="42.25"/>
-    <col customWidth="1" min="3" max="3" width="43.75"/>
-    <col customWidth="1" min="4" max="4" width="79.38"/>
-    <col customWidth="1" min="5" max="5" width="46.0"/>
-    <col customWidth="1" min="6" max="6" width="52.63"/>
-    <col customWidth="1" min="7" max="7" width="82.25"/>
-    <col customWidth="1" min="8" max="8" width="140.75"/>
+    <col min="2" max="2" width="42.1640625" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="79.33203125" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
+    <col min="6" max="6" width="52.6640625" customWidth="1"/>
+    <col min="7" max="7" width="82.1640625" customWidth="1"/>
+    <col min="8" max="8" width="140.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,11 +1029,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -975,7 +1041,7 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -990,14 +1056,14 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3">
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1005,7 +1071,7 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1020,14 +1086,14 @@
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4">
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -1035,7 +1101,7 @@
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1050,13 +1116,13 @@
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -1064,7 +1130,7 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1079,13 +1145,13 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
@@ -1093,7 +1159,7 @@
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1108,13 +1174,13 @@
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -1122,7 +1188,7 @@
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1137,13 +1203,13 @@
       <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -1151,7 +1217,7 @@
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1166,42 +1232,42 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -1209,7 +1275,7 @@
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1224,13 +1290,13 @@
       <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -1238,7 +1304,7 @@
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1253,13 +1319,13 @@
       <c r="H11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>51</v>
@@ -1267,7 +1333,7 @@
       <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1282,13 +1348,13 @@
       <c r="H12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="I12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
@@ -1296,7 +1362,7 @@
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1311,13 +1377,13 @@
       <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="I13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
@@ -1325,7 +1391,7 @@
       <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1340,13 +1406,13 @@
       <c r="H14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="I14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>55</v>
@@ -1354,7 +1420,7 @@
       <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1369,13 +1435,13 @@
       <c r="H15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="I15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>55</v>
@@ -1383,7 +1449,7 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1398,13 +1464,13 @@
       <c r="H16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="I16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
@@ -1412,7 +1478,7 @@
       <c r="C17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1427,30 +1493,30 @@
       <c r="H17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-    </row>
-    <row r="18">
+      <c r="I17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>78</v>
@@ -1458,7 +1524,7 @@
       <c r="C18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1473,30 +1539,30 @@
       <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-    </row>
-    <row r="19">
+      <c r="I18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>78</v>
@@ -1504,7 +1570,7 @@
       <c r="C19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1519,638 +1585,692 @@
       <c r="H19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="10">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="I19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-    </row>
-    <row r="21">
+      <c r="I20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="10">
-        <v>21.0</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="I21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-    </row>
-    <row r="23">
+      <c r="I22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="10">
-        <v>23.0</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="I23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="16"/>
-    </row>
-    <row r="25">
+      <c r="I24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="10">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="I25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-    </row>
-    <row r="27">
+      <c r="I26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="16"/>
-      <c r="Z27" s="16"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="10">
-        <v>27.0</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="I27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="16"/>
-    </row>
-    <row r="29">
+      <c r="I28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="B29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="16"/>
-      <c r="Z29" s="16"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="10">
-        <v>29.0</v>
-      </c>
-      <c r="B30" s="10" t="s">
+      <c r="I29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="16"/>
-      <c r="Z30" s="16"/>
-    </row>
-    <row r="31">
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-    </row>
-    <row r="32">
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-    </row>
-    <row r="33">
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-    </row>
-    <row r="34">
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-    </row>
-    <row r="35">
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-    </row>
-    <row r="37">
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
+      <c r="I30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+    </row>
+    <row r="31" spans="1:26" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="19">
+        <v>30</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
+    </row>
+    <row r="32" spans="1:26" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="19">
+        <v>31</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+    </row>
+    <row r="33" spans="10:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+    </row>
+    <row r="34" spans="10:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="10:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+    </row>
+    <row r="36" spans="10:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" spans="10:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made manual test and refactor, plus npm run format
</commit_message>
<xml_diff>
--- a/worknest-ui/Manual_Tests.xlsx
+++ b/worknest-ui/Manual_Tests.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\SECONDO ANNO MAGISTRALE\SECONDO SEMESTRE\LAB DI PROGETTAZIONE\WorkNest\worknest-ui\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5443150-7090-4FBC-B231-B69B0C86D19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Manual_Tests.csv" sheetId="1" r:id="rId4"/>
+    <sheet name="Manual_Tests.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="183">
   <si>
     <t>Test case ID</t>
   </si>
@@ -486,51 +495,219 @@
     <t>An email arrives to the user after he cancels a booking</t>
   </si>
   <si>
-    <t>1) 1) The user complete the "Cancel Booking" process</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;date&gt;, &lt;workstation name&gt; and in the email is correct and the &lt;rmail object&gt; is "Delete booking confirmed" </t>
   </si>
   <si>
     <t>An email reporting the date of the canceld booking, the relative workstation and a confirmation of the successful deleting arrived to the user</t>
+  </si>
+  <si>
+    <t>WorkNest Administrator Login #58</t>
+  </si>
+  <si>
+    <t>The user wants to log in with his credentials as an admin</t>
+  </si>
+  <si>
+    <t>Buttons for managing users, companies and bookings are shown</t>
+  </si>
+  <si>
+    <t>The user wants to log in with his credentials as a user</t>
+  </si>
+  <si>
+    <t>&lt;email&gt; and &lt;password&gt; are valid and user type is equal to private user</t>
+  </si>
+  <si>
+    <t>The user login in as an administrator</t>
+  </si>
+  <si>
+    <t>The user login in as a user</t>
+  </si>
+  <si>
+    <t>The administrator user is already registered</t>
+  </si>
+  <si>
+    <t>&lt;email&gt; and &lt;password&gt; are valid and user type is equal to administrator</t>
+  </si>
+  <si>
+    <t>Buttons for managing users, companies and bookings (of all users) are not shown</t>
+  </si>
+  <si>
+    <t>The admin wants insert the company in the system and the relative business user</t>
+  </si>
+  <si>
+    <t>The user wants to login as an empolyee of a company</t>
+  </si>
+  <si>
+    <t>The admin inserts all the fileds for the company and for the business user</t>
+  </si>
+  <si>
+    <t>The user inserts a valid company code</t>
+  </si>
+  <si>
+    <t>The user inserts an invalid company code</t>
+  </si>
+  <si>
+    <t>Comapny Registration #26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) The admin is logged in the system </t>
+  </si>
+  <si>
+    <t>1) The admin is logged in the system</t>
+  </si>
+  <si>
+    <t>1) The user complete the "Cancel Booking" process</t>
+  </si>
+  <si>
+    <t>&lt;company&gt; has all field compiled, &lt;business user&gt; has &lt;name&gt;, &lt;surname&gt;, unique &lt;email&gt;, valid &lt;password&gt; compiled</t>
+  </si>
+  <si>
+    <t>The admin not inserts all the field for the company</t>
+  </si>
+  <si>
+    <t>The admin inserts a not valid email for business user or for the company</t>
+  </si>
+  <si>
+    <t>The admin inserts an email already in use for the company or for the business user</t>
+  </si>
+  <si>
+    <t>The admin inserts a not valid password for the business user</t>
+  </si>
+  <si>
+    <t>&lt;company&gt; has not all field compiled</t>
+  </si>
+  <si>
+    <t>A dialog with a succesful message is shown and the business user recives an email with necessary data to make login</t>
+  </si>
+  <si>
+    <t>Error messages are shown under the missings field and submit button isn't clickable</t>
+  </si>
+  <si>
+    <t>The admin inserts 2 different password (password is different from confirm password)</t>
+  </si>
+  <si>
+    <t>&lt;company email&gt; is not valid and/or &lt;business_user email&gt; is not valid</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the sidebar 2) The admin completes the registration form with all valid data 3) The admin clicks on submit</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the sidebar 2) The admin completes partially  the registration form for the company</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the sidebar 2) The admin inserts an invalid email for the company and/or for the business user</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the sidebar 2) The admin inserts an email already in use by the company and/or by the business user</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the siderbar 2) The admin inserts a not valid password</t>
+  </si>
+  <si>
+    <t>1) The admin clicks on "Add new company" in the siderbar 2) The admin inserts two differents passwords</t>
+  </si>
+  <si>
+    <t>Error messages are shown under the email fields and submit button isn't clickable</t>
+  </si>
+  <si>
+    <t>Error message is shown under the confirm password field and submit button isn't clickable</t>
+  </si>
+  <si>
+    <t>Error message is shown under the password field and submit button isn't clickable</t>
+  </si>
+  <si>
+    <t>1) The user clicks "Sign up now" 2) The user inserts a company code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;company code&gt; exists </t>
+  </si>
+  <si>
+    <t>Users submits as an employee for the reltive company</t>
+  </si>
+  <si>
+    <t>&lt;company code&gt; is invalid or doesn't exist</t>
+  </si>
+  <si>
+    <t>User can't submit the form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF2EB452"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -574,156 +751,233 @@
         <bgColor theme="5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F0F3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F0F3"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2EB452"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2EB452"/>
+        <bgColor rgb="FFEC3728"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEC3728"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="40">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE8F0FE"/>
+          <bgColor rgb="FFE8F0FE"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B95F9"/>
           <bgColor rgb="FF5B95F9"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE8F0FE"/>
-          <bgColor rgb="FFE8F0FE"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Manual_Tests.csv-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Manual_Tests.csv-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFEC3728"/>
+      <color rgb="FF2EB452"/>
+      <color rgb="FFE8F0F3"/>
+      <color rgb="FFCCECFF"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I30" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:I31">
   <tableColumns count="9">
-    <tableColumn name="Test case ID" id="1"/>
-    <tableColumn name="User Story" id="2"/>
-    <tableColumn name="Test Case Scenario" id="3"/>
-    <tableColumn name="Test Case" id="4"/>
-    <tableColumn name="Pre-conditions" id="5"/>
-    <tableColumn name="Test Steps" id="6"/>
-    <tableColumn name="Test Data" id="7"/>
-    <tableColumn name="Expected Result" id="8"/>
-    <tableColumn name="Match result" id="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test case ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="User Story"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test Case Scenario"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Test Case"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Pre-conditions"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Test Steps"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Test Data"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Expected Result"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Match result"/>
   </tableColumns>
-  <tableStyleInfo name="Manual_Tests.csv-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Manual_Tests.csv-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -913,29 +1167,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="42.25"/>
-    <col customWidth="1" min="3" max="3" width="43.75"/>
-    <col customWidth="1" min="4" max="4" width="79.38"/>
-    <col customWidth="1" min="5" max="5" width="46.0"/>
-    <col customWidth="1" min="6" max="6" width="52.63"/>
-    <col customWidth="1" min="7" max="7" width="82.25"/>
-    <col customWidth="1" min="8" max="8" width="140.75"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="185" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="105.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="140.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -963,11 +1222,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -975,7 +1234,7 @@
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -990,14 +1249,14 @@
       <c r="H2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3">
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1005,7 +1264,7 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1020,14 +1279,14 @@
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4">
+      <c r="I3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
@@ -1035,7 +1294,7 @@
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1050,13 +1309,13 @@
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="I4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
@@ -1064,7 +1323,7 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1079,13 +1338,13 @@
       <c r="H5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>24</v>
@@ -1093,7 +1352,7 @@
       <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1108,13 +1367,13 @@
       <c r="H6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -1122,7 +1381,7 @@
       <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1137,13 +1396,13 @@
       <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -1151,7 +1410,7 @@
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1166,42 +1425,42 @@
       <c r="H8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -1209,7 +1468,7 @@
       <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1224,13 +1483,13 @@
       <c r="H10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -1238,7 +1497,7 @@
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="29" t="s">
         <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1253,13 +1512,13 @@
       <c r="H11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>51</v>
@@ -1267,7 +1526,7 @@
       <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1282,13 +1541,13 @@
       <c r="H12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="I12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>55</v>
@@ -1296,7 +1555,7 @@
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1311,13 +1570,13 @@
       <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="I13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
@@ -1325,7 +1584,7 @@
       <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -1340,13 +1599,13 @@
       <c r="H14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="I14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>55</v>
@@ -1354,7 +1613,7 @@
       <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>66</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -1369,13 +1628,13 @@
       <c r="H15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="I15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>55</v>
@@ -1383,7 +1642,7 @@
       <c r="C16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -1398,13 +1657,13 @@
       <c r="H16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="I16" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>55</v>
@@ -1412,7 +1671,7 @@
       <c r="C17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -1427,30 +1686,30 @@
       <c r="H17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-    </row>
-    <row r="18">
+      <c r="I17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>78</v>
@@ -1458,7 +1717,7 @@
       <c r="C18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -1473,30 +1732,30 @@
       <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="8"/>
-    </row>
-    <row r="19">
+      <c r="I18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+    </row>
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>78</v>
@@ -1504,7 +1763,7 @@
       <c r="C19" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -1519,638 +1778,918 @@
       <c r="H19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="10">
-        <v>19.0</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="I19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+    </row>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-    </row>
-    <row r="21">
+      <c r="I20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
+    </row>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="B21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-      <c r="Y21" s="16"/>
-      <c r="Z21" s="16"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="10">
-        <v>21.0</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="I21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+    </row>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F22" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="20"/>
-      <c r="U22" s="20"/>
-      <c r="V22" s="20"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="20"/>
-      <c r="Y22" s="20"/>
-      <c r="Z22" s="20"/>
-    </row>
-    <row r="23">
+      <c r="I22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+      <c r="W22" s="15"/>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+      <c r="Z22" s="15"/>
+    </row>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="B23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="I23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="16"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="16"/>
-      <c r="T23" s="16"/>
-      <c r="U23" s="16"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
-      <c r="Z23" s="16"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="10">
-        <v>23.0</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="I23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+    </row>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="16"/>
-    </row>
-    <row r="25">
+      <c r="I24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
+      <c r="V24" s="12"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="12"/>
+      <c r="Z24" s="12"/>
+    </row>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
-      <c r="O25" s="16"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
-      <c r="S25" s="16"/>
-      <c r="T25" s="16"/>
-      <c r="U25" s="16"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
-      <c r="Z25" s="16"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="10">
-        <v>25.0</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="I25" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+      <c r="Y25" s="12"/>
+      <c r="Z25" s="12"/>
+    </row>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>25</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-    </row>
-    <row r="27">
+      <c r="I26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+    </row>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B27" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="16"/>
-      <c r="T27" s="16"/>
-      <c r="U27" s="16"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="16"/>
-      <c r="Z27" s="16"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="10">
-        <v>27.0</v>
-      </c>
-      <c r="B28" s="10" t="s">
+      <c r="I27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="12"/>
+      <c r="Z27" s="12"/>
+    </row>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="16"/>
-      <c r="O28" s="16"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
-      <c r="S28" s="16"/>
-      <c r="T28" s="16"/>
-      <c r="U28" s="16"/>
-      <c r="V28" s="16"/>
-      <c r="W28" s="16"/>
-      <c r="X28" s="16"/>
-      <c r="Y28" s="16"/>
-      <c r="Z28" s="16"/>
-    </row>
-    <row r="29">
+      <c r="I28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
+      <c r="U28" s="12"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
+      <c r="X28" s="12"/>
+      <c r="Y28" s="12"/>
+      <c r="Z28" s="12"/>
+    </row>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="B29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="16"/>
-      <c r="R29" s="16"/>
-      <c r="S29" s="16"/>
-      <c r="T29" s="16"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="16"/>
-      <c r="Y29" s="16"/>
-      <c r="Z29" s="16"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="10">
-        <v>29.0</v>
-      </c>
-      <c r="B30" s="10" t="s">
+      <c r="I29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+      <c r="S29" s="12"/>
+      <c r="T29" s="12"/>
+      <c r="U29" s="12"/>
+      <c r="V29" s="12"/>
+      <c r="W29" s="12"/>
+      <c r="X29" s="12"/>
+      <c r="Y29" s="12"/>
+      <c r="Z29" s="12"/>
+    </row>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>29</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="H30" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="I30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="12"/>
+      <c r="R30" s="12"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="12"/>
+      <c r="U30" s="12"/>
+      <c r="V30" s="12"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="12"/>
+      <c r="Y30" s="12"/>
+      <c r="Z30" s="12"/>
+    </row>
+    <row r="31" spans="1:26" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="19">
+        <v>30</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="I30" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="16"/>
-      <c r="O30" s="16"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
-      <c r="S30" s="16"/>
-      <c r="T30" s="16"/>
-      <c r="U30" s="16"/>
-      <c r="V30" s="16"/>
-      <c r="W30" s="16"/>
-      <c r="X30" s="16"/>
-      <c r="Y30" s="16"/>
-      <c r="Z30" s="16"/>
-    </row>
-    <row r="31">
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-    </row>
-    <row r="32">
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-    </row>
-    <row r="33">
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-    </row>
-    <row r="34">
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="8"/>
-    </row>
-    <row r="35">
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-    </row>
-    <row r="36">
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-    </row>
-    <row r="37">
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
+      <c r="C31" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+      <c r="T31" s="21"/>
+      <c r="U31" s="21"/>
+      <c r="V31" s="21"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+      <c r="Z31" s="21"/>
+    </row>
+    <row r="32" spans="1:26" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19">
+        <v>31</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
+      <c r="W32" s="21"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="21"/>
+    </row>
+    <row r="33" spans="1:26" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="32">
+        <v>32</v>
+      </c>
+      <c r="B33" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
+      <c r="X33" s="35"/>
+      <c r="Y33" s="35"/>
+      <c r="Z33" s="35"/>
+    </row>
+    <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" spans="1:26" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="31">
+        <v>34</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="I35" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+      <c r="L35" s="35"/>
+      <c r="M35" s="35"/>
+      <c r="N35" s="35"/>
+      <c r="O35" s="35"/>
+      <c r="P35" s="35"/>
+      <c r="Q35" s="35"/>
+      <c r="R35" s="35"/>
+    </row>
+    <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" spans="1:26" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="31">
+        <v>36</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="I37" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+      <c r="L37" s="35"/>
+      <c r="M37" s="35"/>
+      <c r="N37" s="35"/>
+      <c r="O37" s="35"/>
+      <c r="P37" s="35"/>
+      <c r="Q37" s="35"/>
+      <c r="R37" s="35"/>
+    </row>
+    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="25">
+        <v>37</v>
+      </c>
+      <c r="B38" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32">
+        <v>38</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="I39" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="25">
+        <v>39</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="G40" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I41" s="26"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new tests ui and manual for start and end date (frontend)
</commit_message>
<xml_diff>
--- a/worknest-ui/Manual_Tests.xlsx
+++ b/worknest-ui/Manual_Tests.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="262">
   <si>
     <t>Test case ID</t>
   </si>
@@ -844,12 +844,62 @@
   <si>
     <t xml:space="preserve">list of &lt;bookings&gt; </t>
   </si>
+  <si>
+    <t>The business user wants to filter the booking list by
+ selecting the start date of the interval</t>
+  </si>
+  <si>
+    <t>The business user clicks on the calendar icon to choose a start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         1) The user enters email and password 2) The user clicks on Login 
+3) The user clicks on the button to see the booking list
+4) The user clicks the calendar icon and choose a date</t>
+  </si>
+  <si>
+    <t>list of &lt;bookings&gt; and date field start date</t>
+  </si>
+  <si>
+    <t>List of all bookings of the company filtered by a start date</t>
+  </si>
+  <si>
+    <t>The business user wants to filter the booking list by
+ selecting the end date of the interval</t>
+  </si>
+  <si>
+    <t>The business user clicks on the calendar icon to choose an end date</t>
+  </si>
+  <si>
+    <t>list of &lt;bookings&gt; and date field end date</t>
+  </si>
+  <si>
+    <t>List of all bookings of the company filtered by an end date</t>
+  </si>
+  <si>
+    <t>The business user wants to filter the booking list by
+ selecting the start date and the end date of the interval</t>
+  </si>
+  <si>
+    <t>The business user clicks on the calendar icon to choose a start date and an end date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         1) The user enters email and password 2) The user clicks on Login 
+3) The user clicks on the button to see the booking list
+4) The user clicks the calendar icon and choose a date for start date
+5) 4) The user clicks the calendar icon and choose a date for end date</t>
+  </si>
+  <si>
+    <t>list of &lt;bookings&gt;,  date field start date, date field end date</t>
+  </si>
+  <si>
+    <t>List of all bookings of the company filtered by the interval (start date &lt;= dates &lt;= end date)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -882,6 +932,10 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF2AA941"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -947,7 +1001,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -974,11 +1028,22 @@
       <top/>
       <bottom/>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="47">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1098,6 +1163,24 @@
     <xf borderId="1" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="4" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1141,7 +1224,7 @@
       <border/>
     </dxf>
   </dxfs>
-  <tableStyles count="3">
+  <tableStyles count="6">
     <tableStyle count="3" pivot="0" name="Manual_Tests.csv-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -1152,6 +1235,18 @@
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
     <tableStyle count="2" pivot="0" name="Manual_Tests.csv-style 3">
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Manual_Tests.csv-style 4">
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Manual_Tests.csv-style 5">
+      <tableStyleElement dxfId="3" type="firstRowStripe"/>
+      <tableStyleElement dxfId="2" type="secondRowStripe"/>
+    </tableStyle>
+    <tableStyle count="2" pivot="0" name="Manual_Tests.csv-style 6">
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
@@ -1199,6 +1294,39 @@
     <tableColumn name="Column3" id="3"/>
   </tableColumns>
   <tableStyleInfo name="Manual_Tests.csv-style 3" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="G57:I57" displayName="Table_4" name="Table_4" id="4">
+  <tableColumns count="3">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Manual_Tests.csv-style 4" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="G58:I58" displayName="Table_5" name="Table_5" id="5">
+  <tableColumns count="3">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Manual_Tests.csv-style 5" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="G59:I59" displayName="Table_6" name="Table_6" id="6">
+  <tableColumns count="3">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
+  </tableColumns>
+  <tableStyleInfo name="Manual_Tests.csv-style 6" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -3996,43 +4124,79 @@
       <c r="Z56" s="21"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
-      <c r="N57" s="21"/>
-      <c r="O57" s="21"/>
-      <c r="P57" s="21"/>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
-      <c r="S57" s="21"/>
-      <c r="T57" s="21"/>
-      <c r="U57" s="21"/>
-      <c r="V57" s="21"/>
-      <c r="W57" s="21"/>
-      <c r="X57" s="21"/>
-      <c r="Y57" s="21"/>
-      <c r="Z57" s="21"/>
-    </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="A57" s="39">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>249</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="G57" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="H57" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="I57" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="46"/>
+      <c r="N57" s="46"/>
+      <c r="O57" s="46"/>
+      <c r="P57" s="46"/>
+      <c r="Q57" s="46"/>
+      <c r="R57" s="46"/>
+      <c r="S57" s="46"/>
+      <c r="T57" s="46"/>
+      <c r="U57" s="46"/>
+      <c r="V57" s="46"/>
+      <c r="W57" s="46"/>
+      <c r="X57" s="46"/>
+      <c r="Y57" s="46"/>
+      <c r="Z57" s="46"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="33">
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="F58" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="G58" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="H58" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="I58" s="32" t="s">
+        <v>16</v>
+      </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
       <c r="L58" s="21"/>
@@ -4052,32 +4216,50 @@
       <c r="Z58" s="21"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4"/>
-      <c r="U59" s="4"/>
-      <c r="V59" s="4"/>
-      <c r="W59" s="4"/>
-      <c r="X59" s="4"/>
-      <c r="Y59" s="4"/>
-      <c r="Z59" s="4"/>
+      <c r="A59" s="39">
+        <v>58.0</v>
+      </c>
+      <c r="B59" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" s="42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D59" s="43" t="s">
+        <v>258</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>230</v>
+      </c>
+      <c r="F59" s="42" t="s">
+        <v>259</v>
+      </c>
+      <c r="G59" s="42" t="s">
+        <v>260</v>
+      </c>
+      <c r="H59" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="I59" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="J59" s="45"/>
+      <c r="K59" s="45"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="46"/>
+      <c r="N59" s="46"/>
+      <c r="O59" s="46"/>
+      <c r="P59" s="46"/>
+      <c r="Q59" s="46"/>
+      <c r="R59" s="46"/>
+      <c r="S59" s="46"/>
+      <c r="T59" s="46"/>
+      <c r="U59" s="46"/>
+      <c r="V59" s="46"/>
+      <c r="W59" s="46"/>
+      <c r="X59" s="46"/>
+      <c r="Y59" s="46"/>
+      <c r="Z59" s="46"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="4"/>
@@ -5265,9 +5447,9 @@
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
       <c r="M102" s="4"/>
       <c r="N102" s="4"/>
       <c r="O102" s="4"/>
@@ -5293,9 +5475,9 @@
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="3"/>
-      <c r="L103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="4"/>
+      <c r="L103" s="4"/>
       <c r="M103" s="4"/>
       <c r="N103" s="4"/>
       <c r="O103" s="4"/>
@@ -30343,71 +30525,18 @@
       <c r="Y997" s="4"/>
       <c r="Z997" s="4"/>
     </row>
-    <row r="998" ht="15.75" customHeight="1">
-      <c r="A998" s="4"/>
-      <c r="B998" s="4"/>
-      <c r="C998" s="4"/>
-      <c r="D998" s="4"/>
-      <c r="E998" s="4"/>
-      <c r="F998" s="4"/>
-      <c r="G998" s="4"/>
-      <c r="H998" s="4"/>
-      <c r="I998" s="4"/>
-      <c r="J998" s="4"/>
-      <c r="K998" s="4"/>
-      <c r="L998" s="4"/>
-      <c r="M998" s="4"/>
-      <c r="N998" s="4"/>
-      <c r="O998" s="4"/>
-      <c r="P998" s="4"/>
-      <c r="Q998" s="4"/>
-      <c r="R998" s="4"/>
-      <c r="S998" s="4"/>
-      <c r="T998" s="4"/>
-      <c r="U998" s="4"/>
-      <c r="V998" s="4"/>
-      <c r="W998" s="4"/>
-      <c r="X998" s="4"/>
-      <c r="Y998" s="4"/>
-      <c r="Z998" s="4"/>
-    </row>
-    <row r="999" ht="15.75" customHeight="1">
-      <c r="A999" s="4"/>
-      <c r="B999" s="4"/>
-      <c r="C999" s="4"/>
-      <c r="D999" s="4"/>
-      <c r="E999" s="4"/>
-      <c r="F999" s="4"/>
-      <c r="G999" s="4"/>
-      <c r="H999" s="4"/>
-      <c r="I999" s="4"/>
-      <c r="J999" s="4"/>
-      <c r="K999" s="4"/>
-      <c r="L999" s="4"/>
-      <c r="M999" s="4"/>
-      <c r="N999" s="4"/>
-      <c r="O999" s="4"/>
-      <c r="P999" s="4"/>
-      <c r="Q999" s="4"/>
-      <c r="R999" s="4"/>
-      <c r="S999" s="4"/>
-      <c r="T999" s="4"/>
-      <c r="U999" s="4"/>
-      <c r="V999" s="4"/>
-      <c r="W999" s="4"/>
-      <c r="X999" s="4"/>
-      <c r="Y999" s="4"/>
-      <c r="Z999" s="4"/>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId5"/>
-    <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
+  <tableParts count="6">
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>